<commit_message>
Lab3 deliverables and scores
</commit_message>
<xml_diff>
--- a/Notas Data Wrangling .xlsx
+++ b/Notas Data Wrangling .xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JR29\Documents\GitHub\data-wrangling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA8AE3D-9F29-43A0-A804-10906ACA7744}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2612133B-F461-4851-A86F-AFEBA1626687}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11505" activeTab="3" xr2:uid="{46607128-50EE-4F7C-8DA4-5EF31434DE3B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11505" activeTab="4" xr2:uid="{46607128-50EE-4F7C-8DA4-5EF31434DE3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Notas Totales" sheetId="1" r:id="rId1"/>
     <sheet name="Lab1" sheetId="2" r:id="rId2"/>
     <sheet name="Lab2" sheetId="3" r:id="rId3"/>
     <sheet name="Lab3" sheetId="4" r:id="rId4"/>
+    <sheet name="Lab4" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="65">
   <si>
     <t>Carné</t>
   </si>
@@ -219,13 +220,10 @@
     <t>Lab #1 - Importar y juntar archivos de Excel</t>
   </si>
   <si>
-    <t>Falta más desarrollo para comprender mejor la información y encontrar más hechos</t>
-  </si>
-  <si>
-    <t>Falta más análisis de la situación y detalle de lo que se está asumiendo con tablas, etc.</t>
-  </si>
-  <si>
     <t>Lab #3 - Distribuidora del Sur, S.A. - Reporte a JD</t>
+  </si>
+  <si>
+    <t>Lab #4 - Consultoría a Inversiones en Energía, S.A. de C.V.</t>
   </si>
 </sst>
 </file>
@@ -1101,7 +1099,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCF6D9A2-0FCC-4F0F-B565-A95C3C6EE056}">
-  <dimension ref="A1:R19"/>
+  <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
@@ -1193,7 +1191,7 @@
       </c>
       <c r="E2" s="12">
         <f>ROUND(VLOOKUP($B2,'Lab3'!$B$4:$H$20,7,FALSE),1)</f>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
@@ -1206,7 +1204,7 @@
       <c r="N2" s="50"/>
       <c r="O2" s="34">
         <f>+SUM(C2:N2)</f>
-        <v>13.6</v>
+        <v>14.1</v>
       </c>
       <c r="P2" s="14"/>
       <c r="Q2" s="35">
@@ -1215,7 +1213,7 @@
       </c>
       <c r="R2" s="59">
         <f>+O2+P2+Q2</f>
-        <v>13.6</v>
+        <v>14.1</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1235,7 +1233,7 @@
       </c>
       <c r="E3" s="12">
         <f>ROUND(VLOOKUP($B3,'Lab3'!$B$4:$H$20,7,FALSE),1)</f>
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
@@ -1248,7 +1246,7 @@
       <c r="N3" s="50"/>
       <c r="O3" s="34">
         <f t="shared" ref="O3:O18" si="0">+SUM(C3:N3)</f>
-        <v>10</v>
+        <v>13.2</v>
       </c>
       <c r="P3" s="14"/>
       <c r="Q3" s="35">
@@ -1257,7 +1255,7 @@
       </c>
       <c r="R3" s="59">
         <f t="shared" ref="R3:R18" si="1">+O3+P3+Q3</f>
-        <v>10</v>
+        <v>13.2</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1361,7 +1359,7 @@
       </c>
       <c r="E6" s="12">
         <f>ROUND(VLOOKUP($B6,'Lab3'!$B$4:$H$20,7,FALSE),1)</f>
-        <v>0</v>
+        <v>3.8</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -1374,7 +1372,7 @@
       <c r="N6" s="50"/>
       <c r="O6" s="34">
         <f t="shared" si="0"/>
-        <v>9.6</v>
+        <v>13.399999999999999</v>
       </c>
       <c r="P6" s="14"/>
       <c r="Q6" s="35">
@@ -1383,7 +1381,7 @@
       </c>
       <c r="R6" s="59">
         <f t="shared" si="1"/>
-        <v>9.6</v>
+        <v>13.399999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1403,7 +1401,7 @@
       </c>
       <c r="E7" s="12">
         <f>ROUND(VLOOKUP($B7,'Lab3'!$B$4:$H$20,7,FALSE),1)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
@@ -1416,7 +1414,7 @@
       <c r="N7" s="50"/>
       <c r="O7" s="34">
         <f t="shared" si="0"/>
-        <v>5.8</v>
+        <v>10.8</v>
       </c>
       <c r="P7" s="14"/>
       <c r="Q7" s="35">
@@ -1425,7 +1423,7 @@
       </c>
       <c r="R7" s="59">
         <f t="shared" si="1"/>
-        <v>5.8</v>
+        <v>10.8</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1445,7 +1443,7 @@
       </c>
       <c r="E8" s="12">
         <f>ROUND(VLOOKUP($B8,'Lab3'!$B$4:$H$20,7,FALSE),1)</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
@@ -1458,7 +1456,7 @@
       <c r="N8" s="50"/>
       <c r="O8" s="34">
         <f t="shared" si="0"/>
-        <v>8.8000000000000007</v>
+        <v>12.3</v>
       </c>
       <c r="P8" s="14"/>
       <c r="Q8" s="35">
@@ -1467,7 +1465,7 @@
       </c>
       <c r="R8" s="59">
         <f t="shared" si="1"/>
-        <v>9.8000000000000007</v>
+        <v>13.3</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1487,7 +1485,7 @@
       </c>
       <c r="E9" s="12">
         <f>ROUND(VLOOKUP($B9,'Lab3'!$B$4:$H$20,7,FALSE),1)</f>
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
@@ -1500,7 +1498,7 @@
       <c r="N9" s="50"/>
       <c r="O9" s="34">
         <f t="shared" si="0"/>
-        <v>8.3000000000000007</v>
+        <v>9</v>
       </c>
       <c r="P9" s="14"/>
       <c r="Q9" s="35">
@@ -1509,7 +1507,7 @@
       </c>
       <c r="R9" s="59">
         <f t="shared" si="1"/>
-        <v>8.3000000000000007</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1613,7 +1611,7 @@
       </c>
       <c r="E12" s="12">
         <f>ROUND(VLOOKUP($B12,'Lab3'!$B$4:$H$20,7,FALSE),1)</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
@@ -1626,7 +1624,7 @@
       <c r="N12" s="50"/>
       <c r="O12" s="34">
         <f t="shared" si="0"/>
-        <v>9.6</v>
+        <v>13.1</v>
       </c>
       <c r="P12" s="14"/>
       <c r="Q12" s="35">
@@ -1635,7 +1633,7 @@
       </c>
       <c r="R12" s="59">
         <f t="shared" si="1"/>
-        <v>9.6</v>
+        <v>13.1</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1655,7 +1653,7 @@
       </c>
       <c r="E13" s="12">
         <f>ROUND(VLOOKUP($B13,'Lab3'!$B$4:$H$20,7,FALSE),1)</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
@@ -1668,7 +1666,7 @@
       <c r="N13" s="50"/>
       <c r="O13" s="34">
         <f t="shared" si="0"/>
-        <v>9.8000000000000007</v>
+        <v>13.3</v>
       </c>
       <c r="P13" s="14"/>
       <c r="Q13" s="35">
@@ -1677,7 +1675,7 @@
       </c>
       <c r="R13" s="59">
         <f t="shared" si="1"/>
-        <v>9.8000000000000007</v>
+        <v>13.3</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1697,7 +1695,7 @@
       </c>
       <c r="E14" s="12">
         <f>ROUND(VLOOKUP($B14,'Lab3'!$B$4:$H$20,7,FALSE),1)</f>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
@@ -1710,7 +1708,7 @@
       <c r="N14" s="50"/>
       <c r="O14" s="34">
         <f t="shared" si="0"/>
-        <v>9.6</v>
+        <v>14.1</v>
       </c>
       <c r="P14" s="14"/>
       <c r="Q14" s="35">
@@ -1719,7 +1717,7 @@
       </c>
       <c r="R14" s="59">
         <f t="shared" si="1"/>
-        <v>9.6</v>
+        <v>14.1</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1739,7 +1737,7 @@
       </c>
       <c r="E15" s="12">
         <f>ROUND(VLOOKUP($B15,'Lab3'!$B$4:$H$20,7,FALSE),1)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
@@ -1752,7 +1750,7 @@
       <c r="N15" s="50"/>
       <c r="O15" s="34">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="P15" s="14"/>
       <c r="Q15" s="35">
@@ -1761,7 +1759,7 @@
       </c>
       <c r="R15" s="59">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1781,7 +1779,7 @@
       </c>
       <c r="E16" s="12">
         <f>ROUND(VLOOKUP($B16,'Lab3'!$B$4:$H$20,7,FALSE),1)</f>
-        <v>4.4000000000000004</v>
+        <v>3.2</v>
       </c>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
@@ -1794,7 +1792,7 @@
       <c r="N16" s="50"/>
       <c r="O16" s="34">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>12.8</v>
       </c>
       <c r="P16" s="14"/>
       <c r="Q16" s="35">
@@ -1803,10 +1801,10 @@
       </c>
       <c r="R16" s="59">
         <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="42" t="s">
         <v>34</v>
       </c>
@@ -1823,7 +1821,7 @@
       </c>
       <c r="E17" s="12">
         <f>ROUND(VLOOKUP($B17,'Lab3'!$B$4:$H$20,7,FALSE),1)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
@@ -1836,7 +1834,7 @@
       <c r="N17" s="50"/>
       <c r="O17" s="34">
         <f t="shared" si="0"/>
-        <v>9.6</v>
+        <v>14.6</v>
       </c>
       <c r="P17" s="14"/>
       <c r="Q17" s="35">
@@ -1845,10 +1843,10 @@
       </c>
       <c r="R17" s="59">
         <f t="shared" si="1"/>
-        <v>11.6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>16.600000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="44" t="s">
         <v>35</v>
       </c>
@@ -1890,7 +1888,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C19" s="8" t="s">
         <v>36</v>
       </c>
@@ -1936,6 +1934,7 @@
       <c r="R19" s="10" t="s">
         <v>50</v>
       </c>
+      <c r="S19" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1950,7 +1949,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2112,12 +2111,23 @@
       <c r="B7" s="17">
         <v>20160281</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
+      <c r="C7" s="18">
+        <v>0</v>
+      </c>
+      <c r="D7" s="18">
+        <v>0</v>
+      </c>
+      <c r="E7" s="18">
+        <v>0</v>
+      </c>
       <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="19"/>
+      <c r="G7" s="18">
+        <v>0</v>
+      </c>
+      <c r="H7" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
@@ -2474,7 +2484,7 @@
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" sqref="A1:R1"/>
@@ -3337,6 +3347,558 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BAEA558-0868-45FE-A870-6EF51C311587}">
+  <dimension ref="A1:I21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="8" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+    </row>
+    <row r="2" spans="1:9" s="21" customFormat="1" ht="57.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="61" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="62" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="21" customFormat="1" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="61"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="H3" s="62"/>
+      <c r="I3" s="39"/>
+    </row>
+    <row r="4" spans="1:9" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="17">
+        <v>20150205</v>
+      </c>
+      <c r="C4" s="18">
+        <v>100</v>
+      </c>
+      <c r="D4" s="18">
+        <v>100</v>
+      </c>
+      <c r="E4" s="18">
+        <v>100</v>
+      </c>
+      <c r="F4" s="18">
+        <v>100</v>
+      </c>
+      <c r="G4" s="18">
+        <v>100</v>
+      </c>
+      <c r="H4" s="19">
+        <f>+SUMPRODUCT($C$3:$G$3,$C4:$G4)/100*5</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="17">
+        <v>20150195</v>
+      </c>
+      <c r="C5" s="18">
+        <v>100</v>
+      </c>
+      <c r="D5" s="18">
+        <v>75</v>
+      </c>
+      <c r="E5" s="18">
+        <v>50</v>
+      </c>
+      <c r="F5" s="18">
+        <v>50</v>
+      </c>
+      <c r="G5" s="18">
+        <v>50</v>
+      </c>
+      <c r="H5" s="19">
+        <f t="shared" ref="H5:H20" si="0">+SUMPRODUCT($C$3:$G$3,$C5:$G5)/100*5</f>
+        <v>3.1875</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="17">
+        <v>20150025</v>
+      </c>
+      <c r="C6" s="18">
+        <v>100</v>
+      </c>
+      <c r="D6" s="18">
+        <v>100</v>
+      </c>
+      <c r="E6" s="18">
+        <v>100</v>
+      </c>
+      <c r="F6" s="18">
+        <v>100</v>
+      </c>
+      <c r="G6" s="18">
+        <v>100</v>
+      </c>
+      <c r="H6" s="19">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="17">
+        <v>20160281</v>
+      </c>
+      <c r="C7" s="18">
+        <v>0</v>
+      </c>
+      <c r="D7" s="18">
+        <v>0</v>
+      </c>
+      <c r="E7" s="18">
+        <v>0</v>
+      </c>
+      <c r="F7" s="18">
+        <v>0</v>
+      </c>
+      <c r="G7" s="18">
+        <v>0</v>
+      </c>
+      <c r="H7" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="17">
+        <v>20130002</v>
+      </c>
+      <c r="C8" s="18">
+        <v>100</v>
+      </c>
+      <c r="D8" s="18">
+        <v>100</v>
+      </c>
+      <c r="E8" s="18">
+        <v>50</v>
+      </c>
+      <c r="F8" s="18">
+        <v>50</v>
+      </c>
+      <c r="G8" s="18">
+        <v>100</v>
+      </c>
+      <c r="H8" s="19">
+        <f t="shared" si="0"/>
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="17">
+        <v>20160090</v>
+      </c>
+      <c r="C9" s="18">
+        <v>100</v>
+      </c>
+      <c r="D9" s="18">
+        <v>100</v>
+      </c>
+      <c r="E9" s="18">
+        <v>100</v>
+      </c>
+      <c r="F9" s="18">
+        <v>100</v>
+      </c>
+      <c r="G9" s="18">
+        <v>100</v>
+      </c>
+      <c r="H9" s="19">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="17">
+        <v>20160825</v>
+      </c>
+      <c r="C10" s="18">
+        <v>100</v>
+      </c>
+      <c r="D10" s="18">
+        <v>100</v>
+      </c>
+      <c r="E10" s="18">
+        <v>50</v>
+      </c>
+      <c r="F10" s="18">
+        <v>50</v>
+      </c>
+      <c r="G10" s="18">
+        <v>50</v>
+      </c>
+      <c r="H10" s="19">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="4">
+        <v>20160165</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
+        <v>50</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0</v>
+      </c>
+      <c r="G11" s="5">
+        <v>20</v>
+      </c>
+      <c r="H11" s="6">
+        <f t="shared" si="0"/>
+        <v>0.72499999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="4">
+        <v>20180190</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0</v>
+      </c>
+      <c r="H12" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="4">
+        <v>20160198</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0</v>
+      </c>
+      <c r="H13" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="4">
+        <v>20150147</v>
+      </c>
+      <c r="C14" s="5">
+        <v>100</v>
+      </c>
+      <c r="D14" s="5">
+        <v>100</v>
+      </c>
+      <c r="E14" s="5">
+        <v>50</v>
+      </c>
+      <c r="F14" s="5">
+        <v>50</v>
+      </c>
+      <c r="G14" s="5">
+        <v>50</v>
+      </c>
+      <c r="H14" s="6">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="4">
+        <v>20160580</v>
+      </c>
+      <c r="C15" s="5">
+        <v>100</v>
+      </c>
+      <c r="D15" s="5">
+        <v>100</v>
+      </c>
+      <c r="E15" s="5">
+        <v>50</v>
+      </c>
+      <c r="F15" s="5">
+        <v>50</v>
+      </c>
+      <c r="G15" s="5">
+        <v>50</v>
+      </c>
+      <c r="H15" s="6">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="4">
+        <v>20150462</v>
+      </c>
+      <c r="C16" s="5">
+        <v>100</v>
+      </c>
+      <c r="D16" s="5">
+        <v>100</v>
+      </c>
+      <c r="E16" s="5">
+        <v>100</v>
+      </c>
+      <c r="F16" s="5">
+        <v>75</v>
+      </c>
+      <c r="G16" s="5">
+        <v>70</v>
+      </c>
+      <c r="H16" s="6">
+        <f t="shared" si="0"/>
+        <v>4.5374999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="4">
+        <v>20160295</v>
+      </c>
+      <c r="C17" s="5">
+        <v>100</v>
+      </c>
+      <c r="D17" s="5">
+        <v>100</v>
+      </c>
+      <c r="E17" s="5">
+        <v>100</v>
+      </c>
+      <c r="F17" s="5">
+        <v>100</v>
+      </c>
+      <c r="G17" s="5">
+        <v>100</v>
+      </c>
+      <c r="H17" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="4">
+        <v>20150066</v>
+      </c>
+      <c r="C18" s="5">
+        <v>100</v>
+      </c>
+      <c r="D18" s="5">
+        <v>75</v>
+      </c>
+      <c r="E18" s="5">
+        <v>50</v>
+      </c>
+      <c r="F18" s="5">
+        <v>50</v>
+      </c>
+      <c r="G18" s="5">
+        <v>50</v>
+      </c>
+      <c r="H18" s="6">
+        <f t="shared" si="0"/>
+        <v>3.1875</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="4">
+        <v>20170481</v>
+      </c>
+      <c r="C19" s="5">
+        <v>100</v>
+      </c>
+      <c r="D19" s="5">
+        <v>100</v>
+      </c>
+      <c r="E19" s="5">
+        <v>100</v>
+      </c>
+      <c r="F19" s="5">
+        <v>100</v>
+      </c>
+      <c r="G19" s="5">
+        <v>100</v>
+      </c>
+      <c r="H19" s="6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="4">
+        <v>20160582</v>
+      </c>
+      <c r="C20" s="5">
+        <v>0</v>
+      </c>
+      <c r="D20" s="5">
+        <v>0</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0</v>
+      </c>
+      <c r="F20" s="5">
+        <v>0</v>
+      </c>
+      <c r="G20" s="5">
+        <v>0</v>
+      </c>
+      <c r="H20" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="H2:H3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72F4AF95-7926-4F81-BE96-4C2C81657B7F}">
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -3358,7 +3920,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="63" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="63"/>
       <c r="C1" s="63"/>
@@ -3413,9 +3975,7 @@
         <v>0.1</v>
       </c>
       <c r="H3" s="62"/>
-      <c r="I3" s="39" t="s">
-        <v>56</v>
-      </c>
+      <c r="I3" s="39"/>
     </row>
     <row r="4" spans="1:9" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="16" t="s">
@@ -3424,27 +3984,14 @@
       <c r="B4" s="17">
         <v>20150205</v>
       </c>
-      <c r="C4" s="18">
-        <v>100</v>
-      </c>
-      <c r="D4" s="18">
-        <v>80</v>
-      </c>
-      <c r="E4" s="18">
-        <v>80</v>
-      </c>
-      <c r="F4" s="18">
-        <v>100</v>
-      </c>
-      <c r="G4" s="18">
-        <v>100</v>
-      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
       <c r="H4" s="19">
         <f>+SUMPRODUCT($C$3:$G$3,$C4:$G4)/100*5</f>
-        <v>4.5</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>63</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3471,24 +4018,14 @@
       <c r="B6" s="17">
         <v>20150025</v>
       </c>
-      <c r="C6" s="18">
-        <v>100</v>
-      </c>
-      <c r="D6" s="18">
-        <v>100</v>
-      </c>
-      <c r="E6" s="18">
-        <v>100</v>
-      </c>
-      <c r="F6" s="18">
-        <v>100</v>
-      </c>
-      <c r="G6" s="18">
-        <v>100</v>
-      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
       <c r="H6" s="19">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3503,7 +4040,10 @@
       <c r="E7" s="18"/>
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
-      <c r="H7" s="19"/>
+      <c r="H7" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
@@ -3658,7 +4198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>32</v>
       </c>
@@ -3675,37 +4215,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="4">
         <v>20150066</v>
       </c>
-      <c r="C18" s="5">
-        <v>100</v>
-      </c>
-      <c r="D18" s="5">
-        <v>75</v>
-      </c>
-      <c r="E18" s="5">
-        <v>100</v>
-      </c>
-      <c r="F18" s="5">
-        <v>75</v>
-      </c>
-      <c r="G18" s="5">
-        <v>100</v>
-      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
       <c r="H18" s="6">
         <f t="shared" si="0"/>
-        <v>4.375</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>34</v>
       </c>
@@ -3722,7 +4249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>35</v>
       </c>
@@ -3739,7 +4266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:H1"/>

</xml_diff>